<commit_message>
handling of row as strign and using split ith "@!@" as parameter to divide in array. Added new file to git ignore
</commit_message>
<xml_diff>
--- a/TextToColumn.xlsx
+++ b/TextToColumn.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -570,17 +570,17 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>asdlkfjiozuxiojsdklfjj#</t>
+          <t>asdlkfjiozuxiojsdklfjj#!@dfax</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>dfax</t>
+          <t>13918771256</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2411/01/25 22:20:56</t>
+          <t>2022-12-29 00:00:00</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -595,15 +595,10 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2022-12-29 00:00:00</t>
+          <t>system</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
-        <is>
-          <t>system</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
         <is>
           <t>system</t>
         </is>
@@ -667,17 +662,17 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>asdlkfjiozuxiojsdklfjj#</t>
+          <t>asdlkfjiozuxiojsdklfjj#!fdsk32x</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>fdsk32x</t>
+          <t>13918771250</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2411/01/25 22:20:50</t>
+          <t>2022-12-29 00:00:00</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -692,15 +687,10 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2022-12-29 00:00:00</t>
+          <t>system</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
-        <is>
-          <t>system</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
         <is>
           <t>system</t>
         </is>

</xml_diff>